<commit_message>
added tbl_user_friend_mst and tbl_friend_request_mst
</commit_message>
<xml_diff>
--- a/erd/ewallet_ERD.xlsx
+++ b/erd/ewallet_ERD.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code Playground\ewallet\erd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rgalpo\Desktop\Files\code playground\ewallet\erd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8313A7A9-0FD7-46C4-B440-CB9151CAFA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{1FD3A013-91EE-462A-B7E3-252B0005E0EF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="58">
   <si>
     <t>tbl_user_mst</t>
   </si>
@@ -175,12 +174,36 @@
   </si>
   <si>
     <t>varchar(10)</t>
+  </si>
+  <si>
+    <t>tbl_user_friend_mst</t>
+  </si>
+  <si>
+    <t>uf_id</t>
+  </si>
+  <si>
+    <t>firend_id</t>
+  </si>
+  <si>
+    <t>tbl_friend_request_mst</t>
+  </si>
+  <si>
+    <t>fr_id</t>
+  </si>
+  <si>
+    <t>block_flag</t>
+  </si>
+  <si>
+    <t>requestee_id</t>
+  </si>
+  <si>
+    <t>requestor_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -216,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -239,19 +262,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2012,6 +2083,805 @@
       <xdr:spPr>
         <a:xfrm rot="5400000">
           <a:off x="10507273" y="7634189"/>
+          <a:ext cx="205740" cy="177362"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>14654</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Rectangle 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C48E8B97-9250-4EA4-B638-C757C45A5F11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="612321" y="5143500"/>
+          <a:ext cx="3960726" cy="183173"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>14654</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Rectangle 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C48E8B97-9250-4EA4-B638-C757C45A5F11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="612321" y="5334000"/>
+          <a:ext cx="3960726" cy="183173"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>14654</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Rectangle 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C48E8B97-9250-4EA4-B638-C757C45A5F11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="612321" y="7048500"/>
+          <a:ext cx="3960726" cy="183173"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>14654</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Rectangle 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C48E8B97-9250-4EA4-B638-C757C45A5F11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="607219" y="7429500"/>
+          <a:ext cx="3949669" cy="183173"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>14654</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>98914</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>27354</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>91587</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Elbow Connector 11"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="30" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4573047" y="670414"/>
+          <a:ext cx="12700" cy="4564673"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2657142"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>177362</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>1633</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Isosceles Triangle 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2893BF1-FC90-E944-7DDC-1360EDED3EA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4544204" y="5144082"/>
+          <a:ext cx="205740" cy="177362"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>14654</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>98914</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>27354</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>91587</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Elbow Connector 17"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="31" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4573047" y="670414"/>
+          <a:ext cx="12700" cy="4755173"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 3728575"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>177362</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Isosceles Triangle 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2893BF1-FC90-E944-7DDC-1360EDED3EA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4544204" y="5348189"/>
+          <a:ext cx="205740" cy="177362"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>98913</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91586</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Elbow Connector 25"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="1"/>
+          <a:endCxn id="32" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="612321" y="670413"/>
+          <a:ext cx="12700" cy="6469673"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1371425"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>505563</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>505563</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Connector 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5FD061B-3665-6A85-ED1F-22DF1ECC7238}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="505563" y="571500"/>
+          <a:ext cx="0" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>432294</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1521</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>7913</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="Isosceles Triangle 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C42EA629-FE2A-41DA-BE1A-F03B4B6164A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="419495" y="7434972"/>
+          <a:ext cx="205740" cy="180141"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>98913</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>91586</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Elbow Connector 34"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="1"/>
+          <a:endCxn id="33" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="608135" y="670413"/>
+          <a:ext cx="12700" cy="6660173"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1890654"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>439620</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>183173</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>8847</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>7913</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="Isosceles Triangle 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C42EA629-FE2A-41DA-BE1A-F03B4B6164A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="425431" y="7245862"/>
           <a:ext cx="205740" cy="177362"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -2350,45 +3220,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE37FC0-3732-4F15-9A76-F3552DFA04CD}">
-  <dimension ref="B2:P47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="K2" s="4" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="K2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -2661,22 +3532,22 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="K13" s="4" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="K13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
@@ -2717,166 +3588,166 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="5" t="s">
+      <c r="G15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="M15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O15" s="5" t="s">
+      <c r="O15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="P15" s="5" t="s">
+      <c r="P15" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="5" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="L16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="M16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="N16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5" t="s">
+      <c r="O16" s="4"/>
+      <c r="P16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" s="5" t="s">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="M17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="N17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5" t="s">
+      <c r="O17" s="4"/>
+      <c r="P17" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="L18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5" t="s">
+      <c r="M18" s="4"/>
+      <c r="N18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5" t="s">
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5" t="s">
+      <c r="M19" s="4"/>
+      <c r="N19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2983,16 +3854,42 @@
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="K25" s="4" t="s">
+      <c r="B25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="K25" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="K26" s="3" t="s">
         <v>1</v>
       </c>
@@ -3013,94 +3910,192 @@
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="K27" s="5" t="s">
+      <c r="B27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="L27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M27" s="5" t="s">
+      <c r="M27" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N27" s="5" t="s">
+      <c r="N27" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O27" s="5" t="s">
+      <c r="O27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="P27" s="5" t="s">
+      <c r="P27" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="K28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N28" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5" t="s">
+      <c r="F28" s="4"/>
+      <c r="G28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="K29" s="5" t="s">
+      <c r="B29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="L29" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M29" s="5" t="s">
+      <c r="M29" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N29" s="5" t="s">
+      <c r="N29" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5" t="s">
+      <c r="O29" s="4"/>
+      <c r="P29" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="K30" s="5" t="s">
+      <c r="B30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="L30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5" t="s">
+      <c r="M30" s="4"/>
+      <c r="N30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="K31" s="5" t="s">
+      <c r="B31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L31" s="5" t="s">
+      <c r="L31" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5" t="s">
+      <c r="M31" s="4"/>
+      <c r="N31" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="K32" s="2" t="s">
         <v>11</v>
       </c>
@@ -3118,7 +4113,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="K33" s="2" t="s">
         <v>12</v>
       </c>
@@ -3136,7 +4147,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K34" s="2" t="s">
         <v>13</v>
       </c>
@@ -3154,17 +4165,63 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="K37" s="4" t="s">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="8"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K37" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-    </row>
-    <row r="38" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="K38" s="3" t="s">
         <v>1</v>
       </c>
@@ -3184,111 +4241,191 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="K39" s="5" t="s">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K39" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="L39" s="5" t="s">
+      <c r="L39" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M39" s="5" t="s">
+      <c r="M39" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N39" s="5" t="s">
+      <c r="N39" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O39" s="5" t="s">
+      <c r="O39" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="P39" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="K40" s="5" t="s">
+      <c r="P39" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L40" s="5" t="s">
+      <c r="L40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M40" s="5" t="s">
+      <c r="M40" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N40" s="5" t="s">
+      <c r="N40" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="K41" s="5" t="s">
+      <c r="O40" s="4"/>
+      <c r="P40" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K41" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L41" s="5" t="s">
+      <c r="L41" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M41" s="5" t="s">
+      <c r="M41" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N41" s="5" t="s">
+      <c r="N41" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="K42" s="5" t="s">
+      <c r="O41" s="4"/>
+      <c r="P41" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K42" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="L42" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="K43" s="5" t="s">
+      <c r="M42" s="4"/>
+      <c r="N42" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K43" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L43" s="5" t="s">
+      <c r="L43" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O43" s="5"/>
-      <c r="P43" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="K44" s="5" t="s">
+      <c r="M43" s="4"/>
+      <c r="N43" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K44" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L44" s="5" t="s">
+      <c r="L44" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5" t="s">
+      <c r="M44" s="4"/>
+      <c r="N44" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K45" s="2" t="s">
         <v>11</v>
       </c>
@@ -3306,7 +4443,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
       <c r="K46" s="2" t="s">
         <v>12</v>
       </c>
@@ -3324,7 +4467,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
       <c r="K47" s="2" t="s">
         <v>13</v>
       </c>
@@ -3342,14 +4491,64 @@
         <v>19</v>
       </c>
     </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="K37:P37"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="K2:P2"/>
     <mergeCell ref="K13:P13"/>
     <mergeCell ref="K25:P25"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B36:G36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>